<commit_message>
Generated image uploaded and stored in db
</commit_message>
<xml_diff>
--- a/public/demo/Updated_create-image.xlsx
+++ b/public/demo/Updated_create-image.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Aman Solution\export-image-with-text\public\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6015E53-24A8-42E1-A70C-9BAA062B436B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B59C84A-303D-4505-8094-2B5021CB77B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,6 @@
     <t>Sr.No.</t>
   </si>
   <si>
-    <t>ProductImage</t>
-  </si>
-  <si>
-    <t>Logo</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>BrandColor</t>
   </si>
   <si>
-    <t>PriceColor</t>
-  </si>
-  <si>
     <t>#000000</t>
   </si>
   <si>
@@ -106,33 +91,12 @@
     <t>#ccc</t>
   </si>
   <si>
-    <t>TextColor</t>
-  </si>
-  <si>
-    <t>TextBackgroundColor</t>
-  </si>
-  <si>
-    <t>PriceBackgroundColor</t>
-  </si>
-  <si>
-    <t>TextFontSize</t>
-  </si>
-  <si>
-    <t>PriceFontSize</t>
-  </si>
-  <si>
     <t>BrandFontSize</t>
   </si>
   <si>
-    <t>TextFontWeight</t>
-  </si>
-  <si>
     <t>BrandFontWeight</t>
   </si>
   <si>
-    <t>PriceFontWeight</t>
-  </si>
-  <si>
     <t>#e63946</t>
   </si>
   <si>
@@ -161,6 +125,42 @@
   </si>
   <si>
     <t>BrandBackgroundColor</t>
+  </si>
+  <si>
+    <t>ProductImageUrl</t>
+  </si>
+  <si>
+    <t>LogoUrl</t>
+  </si>
+  <si>
+    <t>PlanName</t>
+  </si>
+  <si>
+    <t>PriceRange</t>
+  </si>
+  <si>
+    <t>PlanColor</t>
+  </si>
+  <si>
+    <t>PlanBackgroundColor</t>
+  </si>
+  <si>
+    <t>PriceRangeBackgroundColor</t>
+  </si>
+  <si>
+    <t>PriceRangeColor</t>
+  </si>
+  <si>
+    <t>PlanFontSize</t>
+  </si>
+  <si>
+    <t>PriceRangeFontSize</t>
+  </si>
+  <si>
+    <t>PlanFontWeight</t>
+  </si>
+  <si>
+    <t>PriceRangeFontWeight</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -681,15 +681,15 @@
     <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.625" customWidth="1"/>
-    <col min="10" max="10" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,58 +698,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -757,37 +757,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="M2" s="9">
         <v>100</v>
@@ -808,7 +808,7 @@
         <v>700</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -816,37 +816,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M3" s="9">
         <v>100</v>
@@ -867,7 +867,7 @@
         <v>700</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -875,37 +875,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="M4" s="9">
         <v>100</v>
@@ -926,7 +926,7 @@
         <v>700</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -934,37 +934,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="J5" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M5" s="9">
         <v>100</v>
@@ -985,7 +985,7 @@
         <v>700</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A3:F5 A2 F2 C2:D2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A3:F5 A2 F2 C2:D2 F1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>